<commit_message>
Included poscript for india
</commit_message>
<xml_diff>
--- a/WppRegPack/TestResource/EnvParamaters.xlsx
+++ b/WppRegPack/TestResource/EnvParamaters.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\GlobalScript\Master\GlobalTestPack\WppRegPack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\GlobalScript\GlobalTestPack\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="LanguageLookUpTable" sheetId="2" r:id="rId2"/>
-    <sheet name="ServerDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="JIRA_Details" sheetId="4" r:id="rId2"/>
+    <sheet name="JIRAFolderName" sheetId="5" r:id="rId3"/>
+    <sheet name="LanguageLookUpTable" sheetId="2" r:id="rId4"/>
+    <sheet name="ServerDetails" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="354">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -122,6 +124,972 @@
   </si>
   <si>
     <t>TestCycle1</t>
+  </si>
+  <si>
+    <t>IND1-1236</t>
+  </si>
+  <si>
+    <t>CH1-69</t>
+  </si>
+  <si>
+    <t>IND1-1235</t>
+  </si>
+  <si>
+    <t>CH1-77</t>
+  </si>
+  <si>
+    <t>IND1-1234</t>
+  </si>
+  <si>
+    <t>CH1-58</t>
+  </si>
+  <si>
+    <t>IND1-1285</t>
+  </si>
+  <si>
+    <t>CH1-67</t>
+  </si>
+  <si>
+    <t>IND1-1301</t>
+  </si>
+  <si>
+    <t>CH1-42</t>
+  </si>
+  <si>
+    <t>IND1-1293</t>
+  </si>
+  <si>
+    <t>CH1-30</t>
+  </si>
+  <si>
+    <t>04. Changing a Employee</t>
+  </si>
+  <si>
+    <t>IND1-1233</t>
+  </si>
+  <si>
+    <t>CH1-60</t>
+  </si>
+  <si>
+    <t>05. Changing a User</t>
+  </si>
+  <si>
+    <t>IND1-1229</t>
+  </si>
+  <si>
+    <t>CH1-54</t>
+  </si>
+  <si>
+    <t>01. Create Fixed Asset</t>
+  </si>
+  <si>
+    <t>IND1-1237</t>
+  </si>
+  <si>
+    <t>CH1-116</t>
+  </si>
+  <si>
+    <t>02. Posting Asset Adjustment/Entries</t>
+  </si>
+  <si>
+    <t>IND1-1231</t>
+  </si>
+  <si>
+    <t>CH1-119</t>
+  </si>
+  <si>
+    <t>03. Fixed Asset Depreciation</t>
+  </si>
+  <si>
+    <t>IND1-1230</t>
+  </si>
+  <si>
+    <t>CH1-114</t>
+  </si>
+  <si>
+    <t>02. Create SubJobs</t>
+  </si>
+  <si>
+    <t>IND1-1250</t>
+  </si>
+  <si>
+    <t>CH1-62</t>
+  </si>
+  <si>
+    <t>IND1-1248</t>
+  </si>
+  <si>
+    <t>CH1-55</t>
+  </si>
+  <si>
+    <t>04. Modify Budget</t>
+  </si>
+  <si>
+    <t>IND1-1276</t>
+  </si>
+  <si>
+    <t>CH1-137</t>
+  </si>
+  <si>
+    <t>06. Create a Job Quote</t>
+  </si>
+  <si>
+    <t>IND1-1287</t>
+  </si>
+  <si>
+    <t>CH1-135</t>
+  </si>
+  <si>
+    <t>IND1-1269</t>
+  </si>
+  <si>
+    <t>CH1-132</t>
+  </si>
+  <si>
+    <t>IND1-1281</t>
+  </si>
+  <si>
+    <t>CH1-127</t>
+  </si>
+  <si>
+    <t>IND1-1249</t>
+  </si>
+  <si>
+    <t>CH1-128</t>
+  </si>
+  <si>
+    <t>ES02. To Reject a Expense Sheet</t>
+  </si>
+  <si>
+    <t>IND1-1302</t>
+  </si>
+  <si>
+    <t>CH1-43</t>
+  </si>
+  <si>
+    <t>ES03. To Approve a Expense Sheet (OpCo)</t>
+  </si>
+  <si>
+    <t>IND1-1303</t>
+  </si>
+  <si>
+    <t>CH1-40</t>
+  </si>
+  <si>
+    <t>ES04. To Approve a Expense Sheet (SSC)</t>
+  </si>
+  <si>
+    <t>IND1-1304</t>
+  </si>
+  <si>
+    <t>CH1-41</t>
+  </si>
+  <si>
+    <t>TS02. To Reject a Time Sheet Line</t>
+  </si>
+  <si>
+    <t>IND1-1294</t>
+  </si>
+  <si>
+    <t>CH1-31</t>
+  </si>
+  <si>
+    <t>TS03. To Approve a Time Sheet Line</t>
+  </si>
+  <si>
+    <t>IND1-1296</t>
+  </si>
+  <si>
+    <t>CH1-32</t>
+  </si>
+  <si>
+    <t>01. Create a Client</t>
+  </si>
+  <si>
+    <t>IND1-1261</t>
+  </si>
+  <si>
+    <t>CH1-129</t>
+  </si>
+  <si>
+    <t>02. Create a Company Client</t>
+  </si>
+  <si>
+    <t>IND1-1259</t>
+  </si>
+  <si>
+    <t>CH1-121</t>
+  </si>
+  <si>
+    <t>03. Create a Brand</t>
+  </si>
+  <si>
+    <t>IND1-1278</t>
+  </si>
+  <si>
+    <t>CH1-123</t>
+  </si>
+  <si>
+    <t>04. Create a Company Brand</t>
+  </si>
+  <si>
+    <t>IND1-1277</t>
+  </si>
+  <si>
+    <t>CH1-117</t>
+  </si>
+  <si>
+    <t>05. Create a Product</t>
+  </si>
+  <si>
+    <t>IND1-1252</t>
+  </si>
+  <si>
+    <t>CH1-118</t>
+  </si>
+  <si>
+    <t>06. Create a Company Product</t>
+  </si>
+  <si>
+    <t>IND1-1262</t>
+  </si>
+  <si>
+    <t>CH1-110</t>
+  </si>
+  <si>
+    <t>07. Amend a Client</t>
+  </si>
+  <si>
+    <t>IND1-1268</t>
+  </si>
+  <si>
+    <t>CH1-104</t>
+  </si>
+  <si>
+    <t>08. Change a Brand</t>
+  </si>
+  <si>
+    <t>IND1-1280</t>
+  </si>
+  <si>
+    <t>CH1-90</t>
+  </si>
+  <si>
+    <t>01. Create a Vendor (for use by All Companies)</t>
+  </si>
+  <si>
+    <t>IND1-1270</t>
+  </si>
+  <si>
+    <t>CH1-44</t>
+  </si>
+  <si>
+    <t>02. Create a Company Specific Vendor</t>
+  </si>
+  <si>
+    <t>IND1-1272</t>
+  </si>
+  <si>
+    <t>CH1-45</t>
+  </si>
+  <si>
+    <t>03. Change Vendors</t>
+  </si>
+  <si>
+    <t>IND1-1274</t>
+  </si>
+  <si>
+    <t>CH1-46</t>
+  </si>
+  <si>
+    <t>Client Open Statement</t>
+  </si>
+  <si>
+    <t>IND1-1409</t>
+  </si>
+  <si>
+    <t>CH1-103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit Note </t>
+  </si>
+  <si>
+    <t>IND1-1428</t>
+  </si>
+  <si>
+    <t>CH1-138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft Credit Note </t>
+  </si>
+  <si>
+    <t>IND1-1429</t>
+  </si>
+  <si>
+    <t>CH1-139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft Invoice </t>
+  </si>
+  <si>
+    <t>IND1-1430</t>
+  </si>
+  <si>
+    <t>CH1-146</t>
+  </si>
+  <si>
+    <t>Expense Sheet</t>
+  </si>
+  <si>
+    <t>IND1-1354</t>
+  </si>
+  <si>
+    <t>CH1-84</t>
+  </si>
+  <si>
+    <t>General Journal</t>
+  </si>
+  <si>
+    <t>IND1-1388</t>
+  </si>
+  <si>
+    <t>CH1-142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice </t>
+  </si>
+  <si>
+    <t>IND1-1431</t>
+  </si>
+  <si>
+    <t>CH1-147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Budget - Estimate </t>
+  </si>
+  <si>
+    <t>IND1-1425</t>
+  </si>
+  <si>
+    <t>CH1-148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Order Confirmation </t>
+  </si>
+  <si>
+    <t>IND1-1426</t>
+  </si>
+  <si>
+    <t>CH1-140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Quotation </t>
+  </si>
+  <si>
+    <t>IND1-1432</t>
+  </si>
+  <si>
+    <t>CH1-141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Order </t>
+  </si>
+  <si>
+    <t>IND1-1427</t>
+  </si>
+  <si>
+    <t>CH1-149</t>
+  </si>
+  <si>
+    <t>Time Sheet</t>
+  </si>
+  <si>
+    <t>IND1-1356</t>
+  </si>
+  <si>
+    <t>CH1-64</t>
+  </si>
+  <si>
+    <t>Vendor Periodic Statement</t>
+  </si>
+  <si>
+    <t>IND1-1390</t>
+  </si>
+  <si>
+    <t>CH1-65</t>
+  </si>
+  <si>
+    <t>Bank Reconciliation</t>
+  </si>
+  <si>
+    <t>IND1-1381</t>
+  </si>
+  <si>
+    <t>CH1-63</t>
+  </si>
+  <si>
+    <t>Bank Reconciliation in Progress</t>
+  </si>
+  <si>
+    <t>IND1-1367</t>
+  </si>
+  <si>
+    <t>CH1-59</t>
+  </si>
+  <si>
+    <t>Client Periodic Statement</t>
+  </si>
+  <si>
+    <t>IND1-1384</t>
+  </si>
+  <si>
+    <t>CH1-61</t>
+  </si>
+  <si>
+    <t>Payment Listing</t>
+  </si>
+  <si>
+    <t>IND1-1364</t>
+  </si>
+  <si>
+    <t>CH1-124</t>
+  </si>
+  <si>
+    <t>Payment Order</t>
+  </si>
+  <si>
+    <t>IND1-1355</t>
+  </si>
+  <si>
+    <t>CH1-125</t>
+  </si>
+  <si>
+    <t>Payment Selection</t>
+  </si>
+  <si>
+    <t>IND1-1410</t>
+  </si>
+  <si>
+    <t>CH1-136</t>
+  </si>
+  <si>
+    <t>Vendor Open Statement</t>
+  </si>
+  <si>
+    <t>IND1-1357</t>
+  </si>
+  <si>
+    <t>CH1-134</t>
+  </si>
+  <si>
+    <t>GL: Balance Sheet</t>
+  </si>
+  <si>
+    <t>IND1-1403</t>
+  </si>
+  <si>
+    <t>CH1-100</t>
+  </si>
+  <si>
+    <t>GL: BFC Extract</t>
+  </si>
+  <si>
+    <t>GL: Billing &amp; Income</t>
+  </si>
+  <si>
+    <t>GL: Profit &amp; Loss</t>
+  </si>
+  <si>
+    <t>IND1-1369</t>
+  </si>
+  <si>
+    <t>CH1-101</t>
+  </si>
+  <si>
+    <t>GL: Trial Balance Detail</t>
+  </si>
+  <si>
+    <t>IND1-1368</t>
+  </si>
+  <si>
+    <t>CH1-74</t>
+  </si>
+  <si>
+    <t>Jobs: Job Detail</t>
+  </si>
+  <si>
+    <t>IND1-1360</t>
+  </si>
+  <si>
+    <t>CH1-75</t>
+  </si>
+  <si>
+    <t>Jobs: Job Summary</t>
+  </si>
+  <si>
+    <t>IND1-1359</t>
+  </si>
+  <si>
+    <t>CH1-72</t>
+  </si>
+  <si>
+    <t>AP: Employee Expense Sheet</t>
+  </si>
+  <si>
+    <t>IND1-1397</t>
+  </si>
+  <si>
+    <t>CH1-70</t>
+  </si>
+  <si>
+    <t>01. Enter a Vendor Invoice - From Purchase Order (PO)</t>
+  </si>
+  <si>
+    <t>IND1-1300</t>
+  </si>
+  <si>
+    <t>CH1-56</t>
+  </si>
+  <si>
+    <t>02. Invoice Approval (Line Level)</t>
+  </si>
+  <si>
+    <t>IND1-1299</t>
+  </si>
+  <si>
+    <t>CH1-52</t>
+  </si>
+  <si>
+    <t>03. Invoice rejection process</t>
+  </si>
+  <si>
+    <t>IND1-1291</t>
+  </si>
+  <si>
+    <t>CH1-53</t>
+  </si>
+  <si>
+    <t>04. Post Vendor Journal</t>
+  </si>
+  <si>
+    <t>IND1-1290</t>
+  </si>
+  <si>
+    <t>CH1-50</t>
+  </si>
+  <si>
+    <t>05. Reverse an Invoice</t>
+  </si>
+  <si>
+    <t>IND1-1289</t>
+  </si>
+  <si>
+    <t>CH1-51</t>
+  </si>
+  <si>
+    <t>06. Credit Note Processing - With PO</t>
+  </si>
+  <si>
+    <t>IND1-1288</t>
+  </si>
+  <si>
+    <t>CH1-48</t>
+  </si>
+  <si>
+    <t>07. Reverse a Credit Note</t>
+  </si>
+  <si>
+    <t>IND1-1298</t>
+  </si>
+  <si>
+    <t>CH1-49</t>
+  </si>
+  <si>
+    <t>Customer Payment for Single Invoice</t>
+  </si>
+  <si>
+    <t>IND1-1292</t>
+  </si>
+  <si>
+    <t>CH1-133</t>
+  </si>
+  <si>
+    <t>Customer Payments - Multiple Invoices or Partial Payments</t>
+  </si>
+  <si>
+    <t>IND1-1295</t>
+  </si>
+  <si>
+    <t>CH1-126</t>
+  </si>
+  <si>
+    <t>Post a Customer Payment</t>
+  </si>
+  <si>
+    <t>IND1-1283</t>
+  </si>
+  <si>
+    <t>CH1-130</t>
+  </si>
+  <si>
+    <t>Post a Customer Payment in Foreign currency</t>
+  </si>
+  <si>
+    <t>IND1-1284</t>
+  </si>
+  <si>
+    <t>CH1-120</t>
+  </si>
+  <si>
+    <t>Writing Off Bad Debts</t>
+  </si>
+  <si>
+    <t>IND1-1297</t>
+  </si>
+  <si>
+    <t>CH1-122</t>
+  </si>
+  <si>
+    <t>01. Create a General Journal</t>
+  </si>
+  <si>
+    <t>IND1-1405</t>
+  </si>
+  <si>
+    <t>CH1-115</t>
+  </si>
+  <si>
+    <t>02. Create a Reversing General Journal</t>
+  </si>
+  <si>
+    <t>IND1-1402</t>
+  </si>
+  <si>
+    <t>CH1-113</t>
+  </si>
+  <si>
+    <t>04. Post Journal Entries</t>
+  </si>
+  <si>
+    <t>IND1-1400</t>
+  </si>
+  <si>
+    <t>CH1-106</t>
+  </si>
+  <si>
+    <t>05. Reverse a General Journal</t>
+  </si>
+  <si>
+    <t>IND1-1407</t>
+  </si>
+  <si>
+    <t>CH1-109</t>
+  </si>
+  <si>
+    <t>06. Create Currency Journal</t>
+  </si>
+  <si>
+    <t>IND1-1406</t>
+  </si>
+  <si>
+    <t>CH1-102</t>
+  </si>
+  <si>
+    <t>07. Import a Budget Model</t>
+  </si>
+  <si>
+    <t>IND1-1373</t>
+  </si>
+  <si>
+    <t>CH1-105</t>
+  </si>
+  <si>
+    <t>Create an Accrual for a Group of Jobs</t>
+  </si>
+  <si>
+    <t>IND1-1312</t>
+  </si>
+  <si>
+    <t>CH1-96</t>
+  </si>
+  <si>
+    <t>Create an Accrual Job by Job</t>
+  </si>
+  <si>
+    <t>IND1-1308</t>
+  </si>
+  <si>
+    <t>CH1-99</t>
+  </si>
+  <si>
+    <t>Invoice on Account</t>
+  </si>
+  <si>
+    <t>IND1-1318</t>
+  </si>
+  <si>
+    <t>CH1-152</t>
+  </si>
+  <si>
+    <t>Invoice Preparation - Transfer Budget to Invoice On Account</t>
+  </si>
+  <si>
+    <t>IND1-1260</t>
+  </si>
+  <si>
+    <t>CH1-93</t>
+  </si>
+  <si>
+    <t>Invoicing from Budget</t>
+  </si>
+  <si>
+    <t>IND1-1315</t>
+  </si>
+  <si>
+    <t>CH1-87</t>
+  </si>
+  <si>
+    <t>Invoicing Plans - Direct Invoicing</t>
+  </si>
+  <si>
+    <t>IND1-1314</t>
+  </si>
+  <si>
+    <t>CH1-88</t>
+  </si>
+  <si>
+    <t>Invoicing Plans - Invoice on Account</t>
+  </si>
+  <si>
+    <t>CH1-91</t>
+  </si>
+  <si>
+    <t>Job Invoice Allocation (With WIP)</t>
+  </si>
+  <si>
+    <t>IND1-1310</t>
+  </si>
+  <si>
+    <t>CH1-86</t>
+  </si>
+  <si>
+    <t>Job Invoice Allocation (Without WIP)</t>
+  </si>
+  <si>
+    <t>IND1-1255</t>
+  </si>
+  <si>
+    <t>CH1-80</t>
+  </si>
+  <si>
+    <t>Partial Invoicing, Carry Forward</t>
+  </si>
+  <si>
+    <t>IND1-1254</t>
+  </si>
+  <si>
+    <t>CH1-73</t>
+  </si>
+  <si>
+    <t>Partial Invoicing, Write Off</t>
+  </si>
+  <si>
+    <t>IND1-1263</t>
+  </si>
+  <si>
+    <t>CH1-71</t>
+  </si>
+  <si>
+    <t>Time and Material Invoicing</t>
+  </si>
+  <si>
+    <t>IND1-1313</t>
+  </si>
+  <si>
+    <t>CH1-68</t>
+  </si>
+  <si>
+    <t>01. Create a Payment Selection</t>
+  </si>
+  <si>
+    <t>IND1-1311</t>
+  </si>
+  <si>
+    <t>CH1-94</t>
+  </si>
+  <si>
+    <t>02. Change Payment Selection</t>
+  </si>
+  <si>
+    <t>IND1-1309</t>
+  </si>
+  <si>
+    <t>CH1-98</t>
+  </si>
+  <si>
+    <t>03. Create Payment File</t>
+  </si>
+  <si>
+    <t>IND1-1317</t>
+  </si>
+  <si>
+    <t>CH1-89</t>
+  </si>
+  <si>
+    <t>04. Print Payment Remittance</t>
+  </si>
+  <si>
+    <t>IND1-1316</t>
+  </si>
+  <si>
+    <t>CH1-92</t>
+  </si>
+  <si>
+    <t>Test Summary</t>
+  </si>
+  <si>
+    <t>JobCreation</t>
+  </si>
+  <si>
+    <t>Timesheet</t>
+  </si>
+  <si>
+    <t>CreateExpenses</t>
+  </si>
+  <si>
+    <t>EmployeeCreation</t>
+  </si>
+  <si>
+    <t>EmployeeUserCreation</t>
+  </si>
+  <si>
+    <t>CreateUser</t>
+  </si>
+  <si>
+    <t>ApprovePO</t>
+  </si>
+  <si>
+    <t>RejectPurchaseOrder</t>
+  </si>
+  <si>
+    <t>CreateBudget</t>
+  </si>
+  <si>
+    <t>FixedAssetPurchaseOrder</t>
+  </si>
+  <si>
+    <t>CreatePurchaseOrder</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>AKQA - 1201 - AKQA SH</t>
+  </si>
+  <si>
+    <t>VMLY&amp;R - 1322 - Y&amp;R SH</t>
+  </si>
+  <si>
+    <t>Wunderman - 1314 - Agenda SH</t>
+  </si>
+  <si>
+    <t>WPPHQ - 1319 - FinancePlus</t>
+  </si>
+  <si>
+    <t>WHW - 1307 - Sudler China(MDS)</t>
+  </si>
+  <si>
+    <t>Superunion - 1204 - Superunion China</t>
+  </si>
+  <si>
+    <t>Grey - 1213 - Grey SH</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1284 - O&amp;M Agency SH</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1271 - O&amp;M Agency BJ</t>
+  </si>
+  <si>
+    <t>Landor - 1205 - Landor China SH</t>
+  </si>
+  <si>
+    <t>JWT - 1240 - JWT SH</t>
+  </si>
+  <si>
+    <t>GTB - 1228 - GTB China</t>
+  </si>
+  <si>
+    <t>Wunderman - 1315 - Wunderman BJ</t>
+  </si>
+  <si>
+    <t>Wunderman - 1309 - Possible BJ</t>
+  </si>
+  <si>
+    <t>WPPHQ - 1318 - Coretech</t>
+  </si>
+  <si>
+    <t>VMLY&amp;R - 1321 - Y&amp;R BJ</t>
+  </si>
+  <si>
+    <t>VMLY&amp;R - 1301 - VML Social China</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1295 - Soho Marketing BJ</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1289 - RedWasabi</t>
+  </si>
+  <si>
+    <t>Grey - 1216 - Grey DPI GZ</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1285 - Ogilvy Fashion and Lifestyle SH</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1273 - O&amp;M Marketing Communication BJ</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1269 - My David BJ</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1263 - Soho Advertising GZ</t>
+  </si>
+  <si>
+    <t>Grey - 1221 - GZ Grey Star Echo Marketing Communications</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1253 - Marketing Communications Consulting BJ(Redworks)</t>
+  </si>
+  <si>
+    <t>Landor - 1203 - Landor China BJ</t>
+  </si>
+  <si>
+    <t>JWT - 1246 - Mirum SH</t>
+  </si>
+  <si>
+    <t>GTB - 1229 - GTB AP</t>
+  </si>
+  <si>
+    <t>JWT - 1239 - JWT BJ</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1296 - Soho Marketing SH</t>
+  </si>
+  <si>
+    <t>VMLY&amp;R - 1304 - Y&amp;R BJ(Reporting)</t>
+  </si>
+  <si>
+    <t>Grey - 1214 - Grey DPI China(Reporting)</t>
+  </si>
+  <si>
+    <t>Ogilvy - 1330 - Bates SH</t>
+  </si>
+  <si>
+    <t>Folder Name</t>
+  </si>
+  <si>
+    <t>TSTAUTO-1</t>
   </si>
 </sst>
 </file>
@@ -322,7 +1290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -349,6 +1317,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,9 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -721,6 +1688,1397 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>314</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C61" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>198</v>
+      </c>
+      <c r="B63" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>201</v>
+      </c>
+      <c r="B64" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" t="s">
+        <v>205</v>
+      </c>
+      <c r="C65" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>207</v>
+      </c>
+      <c r="B66" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>210</v>
+      </c>
+      <c r="B67" t="s">
+        <v>211</v>
+      </c>
+      <c r="C67" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>213</v>
+      </c>
+      <c r="B68" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>216</v>
+      </c>
+      <c r="B69" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>219</v>
+      </c>
+      <c r="B70" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>222</v>
+      </c>
+      <c r="B71" t="s">
+        <v>223</v>
+      </c>
+      <c r="C71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>225</v>
+      </c>
+      <c r="B72" t="s">
+        <v>226</v>
+      </c>
+      <c r="C72" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>228</v>
+      </c>
+      <c r="B73" t="s">
+        <v>229</v>
+      </c>
+      <c r="C73" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>231</v>
+      </c>
+      <c r="B74" t="s">
+        <v>232</v>
+      </c>
+      <c r="C74" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>234</v>
+      </c>
+      <c r="B75" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>237</v>
+      </c>
+      <c r="B76" t="s">
+        <v>238</v>
+      </c>
+      <c r="C76" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>240</v>
+      </c>
+      <c r="B77" t="s">
+        <v>241</v>
+      </c>
+      <c r="C77" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78" t="s">
+        <v>244</v>
+      </c>
+      <c r="C78" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>246</v>
+      </c>
+      <c r="B79" t="s">
+        <v>247</v>
+      </c>
+      <c r="C79" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>249</v>
+      </c>
+      <c r="B80" t="s">
+        <v>250</v>
+      </c>
+      <c r="C80" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>252</v>
+      </c>
+      <c r="B81" t="s">
+        <v>253</v>
+      </c>
+      <c r="C81" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>255</v>
+      </c>
+      <c r="B82" t="s">
+        <v>256</v>
+      </c>
+      <c r="C82" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>258</v>
+      </c>
+      <c r="B83" t="s">
+        <v>259</v>
+      </c>
+      <c r="C83" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>261</v>
+      </c>
+      <c r="B84" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>264</v>
+      </c>
+      <c r="B85" t="s">
+        <v>265</v>
+      </c>
+      <c r="C85" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>267</v>
+      </c>
+      <c r="B86" t="s">
+        <v>268</v>
+      </c>
+      <c r="C86" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>270</v>
+      </c>
+      <c r="B87" t="s">
+        <v>271</v>
+      </c>
+      <c r="C87" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>273</v>
+      </c>
+      <c r="B88" t="s">
+        <v>274</v>
+      </c>
+      <c r="C88" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>276</v>
+      </c>
+      <c r="B89" t="s">
+        <v>265</v>
+      </c>
+      <c r="C89" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>278</v>
+      </c>
+      <c r="B90" t="s">
+        <v>279</v>
+      </c>
+      <c r="C90" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>281</v>
+      </c>
+      <c r="B91" t="s">
+        <v>282</v>
+      </c>
+      <c r="C91" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>284</v>
+      </c>
+      <c r="B92" t="s">
+        <v>285</v>
+      </c>
+      <c r="C92" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>287</v>
+      </c>
+      <c r="B93" t="s">
+        <v>288</v>
+      </c>
+      <c r="C93" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>290</v>
+      </c>
+      <c r="B94" t="s">
+        <v>291</v>
+      </c>
+      <c r="C94" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>293</v>
+      </c>
+      <c r="B95" t="s">
+        <v>294</v>
+      </c>
+      <c r="C95" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>296</v>
+      </c>
+      <c r="B96" t="s">
+        <v>297</v>
+      </c>
+      <c r="C96" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>299</v>
+      </c>
+      <c r="B97" t="s">
+        <v>300</v>
+      </c>
+      <c r="C97" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>302</v>
+      </c>
+      <c r="B98" t="s">
+        <v>303</v>
+      </c>
+      <c r="C98" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1322</v>
+      </c>
+      <c r="B3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1314</v>
+      </c>
+      <c r="B4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1319</v>
+      </c>
+      <c r="B5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1284</v>
+      </c>
+      <c r="B9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1271</v>
+      </c>
+      <c r="B10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1205</v>
+      </c>
+      <c r="B11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1240</v>
+      </c>
+      <c r="B12" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1315</v>
+      </c>
+      <c r="B14" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1309</v>
+      </c>
+      <c r="B15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1318</v>
+      </c>
+      <c r="B16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1321</v>
+      </c>
+      <c r="B17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1301</v>
+      </c>
+      <c r="B18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1295</v>
+      </c>
+      <c r="B19" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1289</v>
+      </c>
+      <c r="B20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1285</v>
+      </c>
+      <c r="B22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1273</v>
+      </c>
+      <c r="B23" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1269</v>
+      </c>
+      <c r="B24" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1263</v>
+      </c>
+      <c r="B25" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1221</v>
+      </c>
+      <c r="B26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1253</v>
+      </c>
+      <c r="B27" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1203</v>
+      </c>
+      <c r="B28" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1246</v>
+      </c>
+      <c r="B29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1229</v>
+      </c>
+      <c r="B30" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1239</v>
+      </c>
+      <c r="B31" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1296</v>
+      </c>
+      <c r="B32" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1304</v>
+      </c>
+      <c r="B33" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1214</v>
+      </c>
+      <c r="B34" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1330</v>
+      </c>
+      <c r="B35" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -772,7 +3130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>